<commit_message>
Fixed missing values for motorbikes freight (used as taxis). Used same values as for LDV passenger.
</commit_message>
<xml_diff>
--- a/InputData/trans/SDoVPbT/Std Dev of Veh Prices by Technology.xlsx
+++ b/InputData/trans/SDoVPbT/Std Dev of Veh Prices by Technology.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipM\InputData\trans\SDoVPbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Hong Kong\Models\eps-hongkong\InputData\trans\SDoVPbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="23955" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="23955" windowHeight="13110" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2081,7 +2081,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2119,7 +2119,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2511,7 +2510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8875,43 +8874,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>624</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>509</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>511</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>512</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>515</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
         <v>516</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="22" t="s">
         <v>519</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="22" t="s">
         <v>520</v>
       </c>
     </row>
@@ -8931,10 +8930,10 @@
       <c r="E2" s="3">
         <v>206127.38518562954</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>94933107.191416278</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="20">
         <v>94933107.191416278</v>
       </c>
       <c r="H2" s="3">
@@ -8972,10 +8971,10 @@
       <c r="E3" s="3">
         <v>135407.27428151103</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <v>0</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="21">
         <v>0</v>
       </c>
       <c r="H3" s="3">
@@ -9013,10 +9012,10 @@
       <c r="E4" s="3">
         <v>132928.01486984815</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>0</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>0</v>
       </c>
       <c r="H4" s="3">
@@ -9054,10 +9053,10 @@
       <c r="E5" s="18">
         <v>132928.01486984815</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <v>64833333.333333336</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="20">
         <v>64833333.333333336</v>
       </c>
       <c r="H5" s="3">
@@ -9095,10 +9094,10 @@
       <c r="E6" s="3">
         <v>154404.11029915701</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>0</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>0</v>
       </c>
       <c r="H6" s="3">
@@ -9136,10 +9135,10 @@
       <c r="E7" s="3">
         <v>150517.12184581585</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>0</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>0</v>
       </c>
       <c r="H7" s="3">
@@ -9177,10 +9176,10 @@
       <c r="E8" s="3">
         <v>170845.9414873973</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>150462425.18688756</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>150462425.18688756</v>
       </c>
       <c r="H8" s="3">
@@ -9227,7 +9226,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>623</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -9446,7 +9445,9 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9458,7 +9459,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>623</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -9640,26 +9641,33 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="19">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
+      <c r="B7" s="3">
+        <f>'SDoVPbT-psgr'!B2</f>
+        <v>13658.022529814965</v>
+      </c>
+      <c r="C7" s="3">
+        <f>'SDoVPbT-psgr'!C2</f>
+        <v>10302.330516464528</v>
+      </c>
+      <c r="D7" s="3">
+        <f>'SDoVPbT-psgr'!D2</f>
+        <v>8309.8800311829455</v>
+      </c>
+      <c r="E7" s="3">
+        <f>'SDoVPbT-psgr'!E2</f>
+        <v>8807.824444583006</v>
+      </c>
+      <c r="F7" s="3">
+        <f>'SDoVPbT-psgr'!F2</f>
+        <v>10230.832818563998</v>
+      </c>
+      <c r="G7" s="3">
+        <f>'SDoVPbT-psgr'!G2</f>
+        <v>10618.899938992296</v>
+      </c>
+      <c r="H7" s="3">
+        <f>'SDoVPbT-psgr'!H2</f>
+        <v>19285.213920368249</v>
       </c>
     </row>
   </sheetData>
@@ -9668,6 +9676,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9901,32 +9927,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81485E5F-171A-4DBC-AAE6-15B70BABD61F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6F19B1A-62E8-4E65-B6CD-7D496D98FF0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E214856-9EEB-462A-BAD5-E94DA7421785}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E214856-9EEB-462A-BAD5-E94DA7421785}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6F19B1A-62E8-4E65-B6CD-7D496D98FF0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81485E5F-171A-4DBC-AAE6-15B70BABD61F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>